<commit_message>
Fix typos in tables
</commit_message>
<xml_diff>
--- a/data/Boundary_Management_Tables.xlsx
+++ b/data/Boundary_Management_Tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rudolphc/Desktop/Git_Projects/boundary_management_taxonomy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rudolphc/Desktop/Git_Projects/sluseallab/boundary_management_taxonomy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB08C731-3857-3B4E-908A-A459928D471A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27281428-AB96-1D46-B69C-59E6A53E811F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{4C8D9691-51F6-9D47-9215-8766C7783DEA}"/>
+    <workbookView xWindow="8720" yWindow="8580" windowWidth="26900" windowHeight="15140" activeTab="2" xr2:uid="{4C8D9691-51F6-9D47-9215-8766C7783DEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Construct_Definitions" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="582">
   <si>
     <t>Permeability</t>
   </si>
@@ -1448,9 +1448,6 @@
     <t>I am willing to change plans with my friends and family so that I can finish a job assignment</t>
   </si>
   <si>
-    <t>Rangd from .75- .79</t>
-  </si>
-  <si>
     <t>I am willing to take an extended lunch break so that I can deal with responsibilities relating to my family and personal life</t>
   </si>
   <si>
@@ -1559,9 +1556,6 @@
     <t>Work-Related Smartphone Use on Vacation</t>
   </si>
   <si>
-    <t>Chen et al. (2018)</t>
-  </si>
-  <si>
     <t>Respondents were asked whether they used their smartphones during their most recent vacation to search for travel information, to search for other nonwork-related information, to connect to the social networking sites, to read work-related messages or e-mails, or to perform work-related tasks. (p. 6)</t>
   </si>
   <si>
@@ -1655,9 +1649,6 @@
     <t>To what extent do you take members of your family or nonwork friends and companions to company-sponsored or informal work-related gatherings?</t>
   </si>
   <si>
-    <t>Items do not reference flexibility and permeaiblity, therefore only assess permeability</t>
-  </si>
-  <si>
     <t>I never/often take care of nonwork matters while physically at my workplace</t>
   </si>
   <si>
@@ -1803,6 +1794,21 @@
   </si>
   <si>
     <t>I share organizational accomplishments on personally owned social media</t>
+  </si>
+  <si>
+    <t>Ranged from .75-.79</t>
+  </si>
+  <si>
+    <t>Chen et al. (2017)</t>
+  </si>
+  <si>
+    <t>Items do not reference flexibility and permeability, and therefore only assess permeability</t>
+  </si>
+  <si>
+    <t>Choose the Venn diagream tha tbest aligns with participants preferences.</t>
+  </si>
+  <si>
+    <t>N/A (Venn diagram method)</t>
   </si>
 </sst>
 </file>
@@ -2573,7 +2579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9719A7-E68A-8846-97F8-AE1FB1E9099F}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A35"/>
     </sheetView>
   </sheetViews>
@@ -3296,8 +3302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C148E74-EAD7-284B-8295-46C94C2D3ED2}">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView zoomScale="65" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A93"/>
+    <sheetView tabSelected="1" topLeftCell="D74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3361,8 +3367,8 @@
       <c r="G2" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>208</v>
+      <c r="H2" s="8">
+        <v>0.61</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>432</v>
@@ -3768,7 +3774,7 @@
         <v>460</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>461</v>
+        <v>577</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>432</v>
@@ -3794,10 +3800,10 @@
         <v>4</v>
       </c>
       <c r="G17" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>462</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>463</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>432</v>
@@ -3823,10 +3829,10 @@
         <v>4</v>
       </c>
       <c r="G18" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>464</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>465</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>432</v>
@@ -3852,10 +3858,10 @@
         <v>4</v>
       </c>
       <c r="G19" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>466</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>467</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>432</v>
@@ -3881,7 +3887,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H20" s="8">
         <v>0.87</v>
@@ -3910,7 +3916,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H21" s="8">
         <v>0.8</v>
@@ -3939,7 +3945,7 @@
         <v>4</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H22" s="8">
         <v>0.7</v>
@@ -3968,7 +3974,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="H23" s="8">
         <v>0.87</v>
@@ -3997,7 +4003,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H24" s="8">
         <v>0.66</v>
@@ -4026,13 +4032,13 @@
         <v>4</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H25" s="8">
         <v>0.88</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4049,13 +4055,13 @@
         <v>284</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F26" s="8">
         <v>2</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>208</v>
@@ -4078,13 +4084,13 @@
         <v>263</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F27" s="8">
         <v>2</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>208</v>
@@ -4107,13 +4113,13 @@
         <v>264</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F28" s="8">
         <v>4</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H28" s="8">
         <v>0.89</v>
@@ -4136,13 +4142,13 @@
         <v>265</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F29" s="8">
         <v>4</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H29" s="8">
         <v>0.93</v>
@@ -4159,7 +4165,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>201</v>
@@ -4171,10 +4177,10 @@
         <v>5</v>
       </c>
       <c r="G30" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="H30" s="8" t="s">
         <v>481</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>482</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>432</v>
@@ -4188,7 +4194,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>202</v>
@@ -4200,10 +4206,10 @@
         <v>5</v>
       </c>
       <c r="G31" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="H31" s="8" t="s">
         <v>483</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>484</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>432</v>
@@ -4217,7 +4223,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>271</v>
@@ -4229,13 +4235,13 @@
         <v>6</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>208</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4246,7 +4252,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>193</v>
@@ -4258,13 +4264,13 @@
         <v>3</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H33" s="8">
         <v>0.71</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4275,7 +4281,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>252</v>
@@ -4287,7 +4293,7 @@
         <v>6</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H34" s="8">
         <v>0.8</v>
@@ -4304,7 +4310,7 @@
         <v>0</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>249</v>
@@ -4316,7 +4322,7 @@
         <v>6</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H35" s="8">
         <v>0.89</v>
@@ -4333,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>217</v>
@@ -4345,7 +4351,7 @@
         <v>4</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H36" s="8">
         <v>0.84</v>
@@ -4362,7 +4368,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>215</v>
@@ -4374,13 +4380,13 @@
         <v>6</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H37" s="8">
         <v>0.87</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4391,7 +4397,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>206</v>
@@ -4403,7 +4409,7 @@
         <v>4</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H38" s="8">
         <v>0.8</v>
@@ -4420,7 +4426,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>286</v>
@@ -4432,7 +4438,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H39" s="8">
         <v>0.95</v>
@@ -4449,7 +4455,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>188</v>
@@ -4461,7 +4467,7 @@
         <v>3</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="H40" s="8">
         <v>0.95</v>
@@ -4478,25 +4484,25 @@
         <v>0</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D41" s="9" t="s">
+        <v>496</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="F41" s="8">
+        <v>5</v>
+      </c>
+      <c r="G41" s="8" t="s">
         <v>497</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>498</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>499</v>
       </c>
       <c r="H41" s="8" t="s">
         <v>208</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4507,19 +4513,19 @@
         <v>0</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F42" s="8">
         <v>4</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="H42" s="8">
         <v>0.95</v>
@@ -4536,7 +4542,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>212</v>
@@ -4548,13 +4554,13 @@
         <v>5</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="H43" s="8">
         <v>0.72</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4565,7 +4571,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>214</v>
@@ -4577,13 +4583,13 @@
         <v>6</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H44" s="8">
         <v>0.75</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4594,7 +4600,7 @@
         <v>171</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>236</v>
@@ -4606,13 +4612,13 @@
         <v>1</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H45" s="8" t="s">
         <v>208</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4623,10 +4629,10 @@
         <v>171</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>172</v>
@@ -4635,7 +4641,7 @@
         <v>3</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H46" s="8">
         <v>0.73</v>
@@ -4652,7 +4658,7 @@
         <v>171</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>230</v>
@@ -4664,13 +4670,13 @@
         <v>3</v>
       </c>
       <c r="G47" s="10" t="s">
+        <v>509</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="I47" s="8" t="s">
         <v>511</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>512</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4681,7 +4687,7 @@
         <v>171</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>232</v>
@@ -4693,13 +4699,13 @@
         <v>3</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4710,10 +4716,10 @@
         <v>171</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>191</v>
@@ -4722,13 +4728,13 @@
         <v>1</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>208</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4739,7 +4745,7 @@
         <v>171</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>232</v>
@@ -4751,13 +4757,13 @@
         <v>5</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H50" s="8">
         <v>0.8</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4765,10 +4771,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>184</v>
@@ -4780,13 +4786,13 @@
         <v>3</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>208</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4794,10 +4800,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>183</v>
@@ -4809,13 +4815,13 @@
         <v>2</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H52" s="8">
         <v>0.86</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4823,10 +4829,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>262</v>
@@ -4838,7 +4844,7 @@
         <v>5</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>208</v>
@@ -4852,10 +4858,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>282</v>
@@ -4867,7 +4873,7 @@
         <v>4</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H54" s="8" t="s">
         <v>208</v>
@@ -4881,10 +4887,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>259</v>
@@ -4896,7 +4902,7 @@
         <v>5</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H55" s="8" t="s">
         <v>208</v>
@@ -4910,10 +4916,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>261</v>
@@ -4925,7 +4931,7 @@
         <v>5</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="H56" s="8" t="s">
         <v>208</v>
@@ -4939,10 +4945,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>272</v>
@@ -4954,13 +4960,13 @@
         <v>3</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="H57" s="8" t="s">
         <v>208</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>530</v>
+        <v>579</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4968,10 +4974,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>245</v>
@@ -4983,7 +4989,7 @@
         <v>5</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="H58" s="8">
         <v>0.85</v>
@@ -4997,10 +5003,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>247</v>
@@ -5012,7 +5018,7 @@
         <v>5</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="H59" s="8">
         <v>0.81</v>
@@ -5026,10 +5032,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>283</v>
@@ -5041,13 +5047,13 @@
         <v>4</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="H60" s="8" t="s">
         <v>208</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5055,13 +5061,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>258</v>
@@ -5070,7 +5076,7 @@
         <v>2</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="H61" s="8" t="s">
         <v>208</v>
@@ -5084,10 +5090,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>205</v>
@@ -5099,13 +5105,13 @@
         <v>4</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="H62" s="8">
         <v>0.91</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5113,10 +5119,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>203</v>
@@ -5128,13 +5134,13 @@
         <v>4</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="H63" s="8">
         <v>0.94</v>
       </c>
       <c r="I63" s="8" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5142,10 +5148,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>233</v>
@@ -5157,13 +5163,13 @@
         <v>4</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="H64" s="8">
         <v>0.82</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5171,10 +5177,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>219</v>
@@ -5186,7 +5192,7 @@
         <v>7</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="H65" s="8">
         <v>0.87</v>
@@ -5200,10 +5206,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>197</v>
@@ -5215,7 +5221,7 @@
         <v>12</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="H66" s="8">
         <v>0.71</v>
@@ -5229,13 +5235,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>250</v>
@@ -5244,13 +5250,13 @@
         <v>11</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5258,13 +5264,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>250</v>
@@ -5273,13 +5279,13 @@
         <v>11</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5287,10 +5293,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>232</v>
@@ -5302,13 +5308,13 @@
         <v>5</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="H69" s="8">
         <v>0.65</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5316,10 +5322,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>229</v>
@@ -5331,7 +5337,7 @@
         <v>4</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="H70" s="8">
         <v>0.9</v>
@@ -5345,10 +5351,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>189</v>
@@ -5357,10 +5363,10 @@
         <v>190</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="G71" s="8" t="s">
-        <v>208</v>
+        <v>581</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>580</v>
       </c>
       <c r="H71" s="8" t="s">
         <v>208</v>
@@ -5374,10 +5380,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>167</v>
@@ -5389,10 +5395,10 @@
         <v>4</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>552</v>
-      </c>
-      <c r="H72" s="8" t="s">
-        <v>208</v>
+        <v>549</v>
+      </c>
+      <c r="H72" s="8">
+        <v>0.94</v>
       </c>
       <c r="I72" s="8" t="s">
         <v>432</v>
@@ -5403,10 +5409,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>273</v>
@@ -5418,13 +5424,13 @@
         <v>3</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="H73" s="8">
         <v>0.87</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5435,7 +5441,7 @@
         <v>174</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>281</v>
@@ -5447,7 +5453,7 @@
         <v>3</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="H74" s="8" t="s">
         <v>208</v>
@@ -5464,7 +5470,7 @@
         <v>174</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>241</v>
@@ -5476,7 +5482,7 @@
         <v>2</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="H75" s="8" t="s">
         <v>208</v>
@@ -5493,7 +5499,7 @@
         <v>174</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>224</v>
@@ -5505,7 +5511,7 @@
         <v>1</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="H76" s="8" t="s">
         <v>208</v>
@@ -5522,7 +5528,7 @@
         <v>174</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>225</v>
@@ -5534,7 +5540,7 @@
         <v>1</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="H77" s="8" t="s">
         <v>208</v>
@@ -5551,7 +5557,7 @@
         <v>174</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>175</v>
@@ -5563,7 +5569,7 @@
         <v>2</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="H78" s="8" t="s">
         <v>208</v>
@@ -5580,7 +5586,7 @@
         <v>174</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>196</v>
@@ -5592,7 +5598,7 @@
         <v>6</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="H79" s="8">
         <v>0.9</v>
@@ -5609,7 +5615,7 @@
         <v>174</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>288</v>
@@ -5621,7 +5627,7 @@
         <v>1</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="H80" s="8" t="s">
         <v>208</v>
@@ -5638,7 +5644,7 @@
         <v>174</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>223</v>
@@ -5650,7 +5656,7 @@
         <v>1</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="H81" s="8" t="s">
         <v>208</v>
@@ -5667,7 +5673,7 @@
         <v>174</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>268</v>
@@ -5679,7 +5685,7 @@
         <v>3</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="H82" s="8">
         <v>0.56000000000000005</v>
@@ -5696,7 +5702,7 @@
         <v>174</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>280</v>
@@ -5708,7 +5714,7 @@
         <v>6</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="H83" s="8" t="s">
         <v>208</v>
@@ -5725,7 +5731,7 @@
         <v>174</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>238</v>
@@ -5737,7 +5743,7 @@
         <v>1</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="H84" s="8" t="s">
         <v>208</v>
@@ -5754,7 +5760,7 @@
         <v>174</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>226</v>
@@ -5766,7 +5772,7 @@
         <v>7</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="H85" s="8" t="s">
         <v>208</v>
@@ -5783,7 +5789,7 @@
         <v>174</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>270</v>
@@ -5795,7 +5801,7 @@
         <v>2</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="H86" s="8">
         <v>0.79</v>
@@ -5812,7 +5818,7 @@
         <v>174</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>266</v>
@@ -5824,7 +5830,7 @@
         <v>3</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H87" s="8">
         <v>0.85</v>
@@ -5841,7 +5847,7 @@
         <v>174</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>266</v>
@@ -5853,7 +5859,7 @@
         <v>10</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="H88" s="8">
         <v>0.91</v>
@@ -5870,10 +5876,10 @@
         <v>174</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E89" s="8" t="s">
         <v>228</v>
@@ -5882,7 +5888,7 @@
         <v>4</v>
       </c>
       <c r="G89" s="8" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="H89" s="8">
         <v>0.83</v>
@@ -5899,7 +5905,7 @@
         <v>174</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>274</v>
@@ -5911,7 +5917,7 @@
         <v>3</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="H90" s="8">
         <v>0.94</v>
@@ -5928,19 +5934,19 @@
         <v>174</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D91" s="32" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="E91" s="32" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="F91" s="30">
         <v>4</v>
       </c>
       <c r="G91" s="34" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="H91" s="30">
         <v>0.83</v>
@@ -5957,7 +5963,7 @@
         <v>174</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D92" s="33"/>
       <c r="E92" s="33"/>
@@ -5974,19 +5980,19 @@
         <v>174</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="F93" s="8">
         <v>6</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="H93" s="8">
         <v>0.93</v>
@@ -6013,7 +6019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10180BE9-1079-A845-8A7C-CC59A2B3DC8C}">
   <dimension ref="A1:N329"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>

</xml_diff>